<commit_message>
Fix Test ID 152
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111AFEAXX/Afea_srl/H2O/6.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111AFEAXX/Afea_srl/H2O/6.0/report-checklist.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2316" uniqueCount="938">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -13335,9 +13335,7 @@
       <c r="F159" s="35"/>
       <c r="G159" s="34"/>
       <c r="H159" s="34"/>
-      <c r="I159" s="35" t="s">
-        <v>69</v>
-      </c>
+      <c r="I159" s="34"/>
       <c r="J159" s="35" t="s">
         <v>69</v>
       </c>
@@ -25895,7 +25893,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10:J36 L10:M36 O10:O36 J38 L38:M38 O38 J40:J43 L40:M44 O40:O44 J46 L46:M46 O46 J48:J52 L48:M52 O48:O52 L54:M77 J54:J158 L79:M158 I159:J159 J160:J198 L160:M198 O54:O198 J375:J383 L375:M383 O375:O383">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10:J36 L10:M36 O10:O36 J38 L38:M38 O38 J40:J43 L40:M44 O40:O44 J46 L46:M46 O46 J48:J52 L48:M52 O48:O52 L54:M77 L79:M158 J54:J198 L160:M198 O54:O198 J375:J383 L375:M383 O375:O383">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q10:Q36 Q38 Q40:Q44 Q46 Q48:Q52 Q54:Q198 Q375:Q383">

</xml_diff>